<commit_message>
Added multi-model document processing and CSV export feature
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,45 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
-  <si>
-    <t>Invoice No</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Party Name</t>
-  </si>
-  <si>
-    <t>HS Code</t>
-  </si>
-  <si>
-    <t>INV-2025-619</t>
-  </si>
-  <si>
-    <t>INV-2025-797</t>
-  </si>
-  <si>
-    <t>INV-2025-947</t>
-  </si>
-  <si>
-    <t>12/8/2025</t>
-  </si>
-  <si>
-    <t>16/5/2025</t>
-  </si>
-  <si>
-    <t>26/12/2025</t>
-  </si>
-  <si>
-    <t>Vista Exports Ltd.</t>
-  </si>
-  <si>
-    <t>Pinnacle Supplies</t>
-  </si>
-  <si>
-    <t>620322</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Place of Issue</t>
+  </si>
+  <si>
+    <t>Date of Issue</t>
+  </si>
+  <si>
+    <t>Date of Expiry</t>
+  </si>
+  <si>
+    <t>Suresh Sharma</t>
+  </si>
+  <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>01/10/1999</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>14/08/2023</t>
+  </si>
+  <si>
+    <t>11/08/2033</t>
   </si>
 </sst>
 </file>
@@ -410,13 +413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,47 +432,42 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>